<commit_message>
Arquivo atualizado Projeto Integrador
</commit_message>
<xml_diff>
--- a/documentacao/5.OrganogramaInsighLab.xlsx
+++ b/documentacao/5.OrganogramaInsighLab.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\2 ESTUDO\20 FATEC 2S2024\PDC011_PROJETO_INTEGRADOR\projetoGrupo05\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0791EAA4-9554-4972-B75C-A5447C5F7C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F34908E-8B54-4E67-BDA6-3D38C65B1E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0759B0C1-0AB1-4BDF-A422-1E59695B969C}"/>
   </bookViews>
@@ -75,17 +75,15 @@
 </file>
 
 <file path=xl/diagrams/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<dgm:colorsDef xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uniqueId="urn:microsoft.com/office/officeart/2005/8/colors/accent5_3">
+<dgm:colorsDef xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uniqueId="urn:microsoft.com/office/officeart/2005/8/colors/accent1_2">
   <dgm:title val=""/>
   <dgm:desc val=""/>
   <dgm:catLst>
-    <dgm:cat type="accent5" pri="11300"/>
+    <dgm:cat type="accent1" pri="11200"/>
   </dgm:catLst>
   <dgm:styleLbl name="node0">
     <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent5">
-        <a:shade val="80000"/>
-      </a:schemeClr>
+      <a:schemeClr val="accent1"/>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
       <a:schemeClr val="lt1"/>
@@ -95,14 +93,21 @@
     <dgm:txFillClrLst/>
     <dgm:txEffectClrLst/>
   </dgm:styleLbl>
+  <dgm:styleLbl name="alignNode1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
   <dgm:styleLbl name="node1">
-    <dgm:fillClrLst>
-      <a:schemeClr val="accent5">
-        <a:shade val="80000"/>
-      </a:schemeClr>
-      <a:schemeClr val="accent5">
-        <a:tint val="70000"/>
-      </a:schemeClr>
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
       <a:schemeClr val="lt1"/>
@@ -112,36 +117,9 @@
     <dgm:txFillClrLst/>
     <dgm:txEffectClrLst/>
   </dgm:styleLbl>
-  <dgm:styleLbl name="alignNode1">
-    <dgm:fillClrLst>
-      <a:schemeClr val="accent5">
-        <a:shade val="80000"/>
-      </a:schemeClr>
-      <a:schemeClr val="accent5">
-        <a:tint val="70000"/>
-      </a:schemeClr>
-    </dgm:fillClrLst>
-    <dgm:linClrLst>
-      <a:schemeClr val="accent5">
-        <a:shade val="80000"/>
-      </a:schemeClr>
-      <a:schemeClr val="accent5">
-        <a:tint val="70000"/>
-      </a:schemeClr>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst/>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
   <dgm:styleLbl name="lnNode1">
-    <dgm:fillClrLst>
-      <a:schemeClr val="accent5">
-        <a:shade val="80000"/>
-      </a:schemeClr>
-      <a:schemeClr val="accent5">
-        <a:tint val="70000"/>
-      </a:schemeClr>
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
       <a:schemeClr val="lt1"/>
@@ -152,13 +130,8 @@
     <dgm:txEffectClrLst/>
   </dgm:styleLbl>
   <dgm:styleLbl name="vennNode1">
-    <dgm:fillClrLst>
-      <a:schemeClr val="accent5">
-        <a:shade val="80000"/>
-        <a:alpha val="50000"/>
-      </a:schemeClr>
-      <a:schemeClr val="accent5">
-        <a:tint val="70000"/>
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
         <a:alpha val="50000"/>
       </a:schemeClr>
     </dgm:fillClrLst>
@@ -171,10 +144,8 @@
     <dgm:txEffectClrLst/>
   </dgm:styleLbl>
   <dgm:styleLbl name="node2">
-    <dgm:fillClrLst>
-      <a:schemeClr val="accent5">
-        <a:tint val="99000"/>
-      </a:schemeClr>
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
       <a:schemeClr val="lt1"/>
@@ -185,10 +156,8 @@
     <dgm:txEffectClrLst/>
   </dgm:styleLbl>
   <dgm:styleLbl name="node3">
-    <dgm:fillClrLst>
-      <a:schemeClr val="accent5">
-        <a:tint val="80000"/>
-      </a:schemeClr>
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
       <a:schemeClr val="lt1"/>
@@ -199,10 +168,8 @@
     <dgm:txEffectClrLst/>
   </dgm:styleLbl>
   <dgm:styleLbl name="node4">
-    <dgm:fillClrLst>
-      <a:schemeClr val="accent5">
-        <a:tint val="70000"/>
-      </a:schemeClr>
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
       <a:schemeClr val="lt1"/>
@@ -213,12 +180,9 @@
     <dgm:txEffectClrLst/>
   </dgm:styleLbl>
   <dgm:styleLbl name="fgImgPlace1">
-    <dgm:fillClrLst>
-      <a:schemeClr val="accent5">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
         <a:tint val="50000"/>
-      </a:schemeClr>
-      <a:schemeClr val="accent5">
-        <a:tint val="20000"/>
       </a:schemeClr>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
@@ -232,12 +196,9 @@
     <dgm:txEffectClrLst/>
   </dgm:styleLbl>
   <dgm:styleLbl name="alignImgPlace1">
-    <dgm:fillClrLst>
-      <a:schemeClr val="accent5">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
         <a:tint val="50000"/>
-      </a:schemeClr>
-      <a:schemeClr val="accent5">
-        <a:tint val="20000"/>
       </a:schemeClr>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
@@ -251,12 +212,9 @@
     <dgm:txEffectClrLst/>
   </dgm:styleLbl>
   <dgm:styleLbl name="bgImgPlace1">
-    <dgm:fillClrLst>
-      <a:schemeClr val="accent5">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
         <a:tint val="50000"/>
-      </a:schemeClr>
-      <a:schemeClr val="accent5">
-        <a:tint val="20000"/>
       </a:schemeClr>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
@@ -270,20 +228,14 @@
     <dgm:txEffectClrLst/>
   </dgm:styleLbl>
   <dgm:styleLbl name="sibTrans2D1">
-    <dgm:fillClrLst>
-      <a:schemeClr val="accent5">
-        <a:shade val="90000"/>
-      </a:schemeClr>
-      <a:schemeClr val="accent5">
-        <a:tint val="70000"/>
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
       </a:schemeClr>
     </dgm:fillClrLst>
-    <dgm:linClrLst>
-      <a:schemeClr val="accent5">
-        <a:shade val="90000"/>
-      </a:schemeClr>
-      <a:schemeClr val="accent5">
-        <a:tint val="70000"/>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
       </a:schemeClr>
     </dgm:linClrLst>
     <dgm:effectClrLst/>
@@ -292,68 +244,58 @@
     <dgm:txEffectClrLst/>
   </dgm:styleLbl>
   <dgm:styleLbl name="fgSibTrans2D1">
-    <dgm:fillClrLst>
-      <a:schemeClr val="accent5">
-        <a:shade val="90000"/>
-      </a:schemeClr>
-      <a:schemeClr val="accent5">
-        <a:tint val="70000"/>
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
       </a:schemeClr>
     </dgm:fillClrLst>
-    <dgm:linClrLst>
-      <a:schemeClr val="accent5">
-        <a:shade val="90000"/>
-      </a:schemeClr>
-      <a:schemeClr val="accent5">
-        <a:tint val="70000"/>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
       </a:schemeClr>
     </dgm:linClrLst>
     <dgm:effectClrLst/>
     <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:txFillClrLst>
+    <dgm:txFillClrLst/>
     <dgm:txEffectClrLst/>
   </dgm:styleLbl>
   <dgm:styleLbl name="bgSibTrans2D1">
-    <dgm:fillClrLst>
-      <a:schemeClr val="accent5">
-        <a:shade val="90000"/>
-      </a:schemeClr>
-      <a:schemeClr val="accent5">
-        <a:tint val="70000"/>
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
       </a:schemeClr>
     </dgm:fillClrLst>
-    <dgm:linClrLst>
-      <a:schemeClr val="accent5">
-        <a:shade val="90000"/>
-      </a:schemeClr>
-      <a:schemeClr val="accent5">
-        <a:tint val="70000"/>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
       </a:schemeClr>
     </dgm:linClrLst>
     <dgm:effectClrLst/>
     <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="sibTrans1D1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
     <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </dgm:txFillClrLst>
     <dgm:txEffectClrLst/>
   </dgm:styleLbl>
-  <dgm:styleLbl name="sibTrans1D1">
-    <dgm:fillClrLst>
-      <a:schemeClr val="accent5">
-        <a:shade val="90000"/>
-      </a:schemeClr>
-      <a:schemeClr val="accent5">
-        <a:tint val="70000"/>
-      </a:schemeClr>
+  <dgm:styleLbl name="callout">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
     </dgm:fillClrLst>
-    <dgm:linClrLst>
-      <a:schemeClr val="accent5">
-        <a:shade val="90000"/>
-      </a:schemeClr>
-      <a:schemeClr val="accent5">
-        <a:tint val="70000"/>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="50000"/>
       </a:schemeClr>
     </dgm:linClrLst>
     <dgm:effectClrLst/>
@@ -363,25 +305,9 @@
     </dgm:txFillClrLst>
     <dgm:txEffectClrLst/>
   </dgm:styleLbl>
-  <dgm:styleLbl name="callout">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent5"/>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent5"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="tx1"/>
-    </dgm:txFillClrLst>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
   <dgm:styleLbl name="asst0">
     <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent5">
-        <a:shade val="80000"/>
-      </a:schemeClr>
+      <a:schemeClr val="accent1"/>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
       <a:schemeClr val="lt1"/>
@@ -393,9 +319,7 @@
   </dgm:styleLbl>
   <dgm:styleLbl name="asst1">
     <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent5">
-        <a:shade val="80000"/>
-      </a:schemeClr>
+      <a:schemeClr val="accent1"/>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
       <a:schemeClr val="lt1"/>
@@ -406,10 +330,8 @@
     <dgm:txEffectClrLst/>
   </dgm:styleLbl>
   <dgm:styleLbl name="asst2">
-    <dgm:fillClrLst>
-      <a:schemeClr val="accent5">
-        <a:tint val="99000"/>
-      </a:schemeClr>
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
       <a:schemeClr val="lt1"/>
@@ -420,10 +342,8 @@
     <dgm:txEffectClrLst/>
   </dgm:styleLbl>
   <dgm:styleLbl name="asst3">
-    <dgm:fillClrLst>
-      <a:schemeClr val="accent5">
-        <a:tint val="80000"/>
-      </a:schemeClr>
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
       <a:schemeClr val="lt1"/>
@@ -434,10 +354,8 @@
     <dgm:txEffectClrLst/>
   </dgm:styleLbl>
   <dgm:styleLbl name="asst4">
-    <dgm:fillClrLst>
-      <a:schemeClr val="accent5">
-        <a:tint val="70000"/>
-      </a:schemeClr>
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
       <a:schemeClr val="lt1"/>
@@ -449,12 +367,12 @@
   </dgm:styleLbl>
   <dgm:styleLbl name="parChTrans2D1">
     <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent5">
+      <a:schemeClr val="accent1">
         <a:tint val="60000"/>
       </a:schemeClr>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent5">
+      <a:schemeClr val="accent1">
         <a:tint val="60000"/>
       </a:schemeClr>
     </dgm:linClrLst>
@@ -467,46 +385,10 @@
   </dgm:styleLbl>
   <dgm:styleLbl name="parChTrans2D2">
     <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent5">
-        <a:tint val="90000"/>
-      </a:schemeClr>
+      <a:schemeClr val="accent1"/>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent5">
-        <a:tint val="90000"/>
-      </a:schemeClr>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst/>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="parChTrans2D3">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent5">
-        <a:tint val="70000"/>
-      </a:schemeClr>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent5">
-        <a:tint val="70000"/>
-      </a:schemeClr>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst/>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="parChTrans2D4">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent5">
-        <a:tint val="50000"/>
-      </a:schemeClr>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent5">
-        <a:tint val="50000"/>
-      </a:schemeClr>
+      <a:schemeClr val="accent1"/>
     </dgm:linClrLst>
     <dgm:effectClrLst/>
     <dgm:txLinClrLst/>
@@ -515,14 +397,72 @@
     </dgm:txFillClrLst>
     <dgm:txEffectClrLst/>
   </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D3">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D4">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
   <dgm:styleLbl name="parChTrans1D1">
     <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent5">
-        <a:shade val="80000"/>
-      </a:schemeClr>
+      <a:schemeClr val="accent1"/>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent5">
+      <a:schemeClr val="accent1">
+        <a:shade val="60000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="tx1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D2">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:shade val="60000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="tx1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D3">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
         <a:shade val="80000"/>
       </a:schemeClr>
     </dgm:linClrLst>
@@ -533,15 +473,13 @@
     </dgm:txFillClrLst>
     <dgm:txEffectClrLst/>
   </dgm:styleLbl>
-  <dgm:styleLbl name="parChTrans1D2">
+  <dgm:styleLbl name="parChTrans1D4">
     <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent5">
-        <a:tint val="99000"/>
-      </a:schemeClr>
+      <a:schemeClr val="accent1"/>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent5">
-        <a:tint val="99000"/>
+      <a:schemeClr val="accent1">
+        <a:shade val="80000"/>
       </a:schemeClr>
     </dgm:linClrLst>
     <dgm:effectClrLst/>
@@ -551,55 +489,14 @@
     </dgm:txFillClrLst>
     <dgm:txEffectClrLst/>
   </dgm:styleLbl>
-  <dgm:styleLbl name="parChTrans1D3">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent5">
-        <a:tint val="80000"/>
-      </a:schemeClr>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent5">
-        <a:tint val="80000"/>
-      </a:schemeClr>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="tx1"/>
-    </dgm:txFillClrLst>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="parChTrans1D4">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent5">
-        <a:tint val="70000"/>
-      </a:schemeClr>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent5">
-        <a:tint val="70000"/>
-      </a:schemeClr>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="tx1"/>
-    </dgm:txFillClrLst>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
   <dgm:styleLbl name="fgAcc1">
     <dgm:fillClrLst meth="repeat">
       <a:schemeClr val="lt1">
         <a:alpha val="90000"/>
       </a:schemeClr>
     </dgm:fillClrLst>
-    <dgm:linClrLst>
-      <a:schemeClr val="accent5">
-        <a:shade val="80000"/>
-      </a:schemeClr>
-      <a:schemeClr val="accent5">
-        <a:tint val="70000"/>
-      </a:schemeClr>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
     </dgm:linClrLst>
     <dgm:effectClrLst/>
     <dgm:txLinClrLst/>
@@ -614,13 +511,8 @@
         <a:alpha val="90000"/>
       </a:schemeClr>
     </dgm:fillClrLst>
-    <dgm:linClrLst>
-      <a:schemeClr val="accent5">
-        <a:shade val="80000"/>
-      </a:schemeClr>
-      <a:schemeClr val="accent5">
-        <a:tint val="70000"/>
-      </a:schemeClr>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
     </dgm:linClrLst>
     <dgm:effectClrLst/>
     <dgm:txLinClrLst/>
@@ -635,13 +527,8 @@
         <a:alpha val="90000"/>
       </a:schemeClr>
     </dgm:fillClrLst>
-    <dgm:linClrLst>
-      <a:schemeClr val="accent5">
-        <a:shade val="80000"/>
-      </a:schemeClr>
-      <a:schemeClr val="accent5">
-        <a:tint val="70000"/>
-      </a:schemeClr>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
     </dgm:linClrLst>
     <dgm:effectClrLst/>
     <dgm:txLinClrLst/>
@@ -657,7 +544,7 @@
       </a:schemeClr>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent5"/>
+      <a:schemeClr val="accent1"/>
     </dgm:linClrLst>
     <dgm:effectClrLst/>
     <dgm:txLinClrLst/>
@@ -672,13 +559,8 @@
         <a:alpha val="90000"/>
       </a:schemeClr>
     </dgm:fillClrLst>
-    <dgm:linClrLst>
-      <a:schemeClr val="accent5">
-        <a:shade val="80000"/>
-      </a:schemeClr>
-      <a:schemeClr val="accent5">
-        <a:tint val="70000"/>
-      </a:schemeClr>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
     </dgm:linClrLst>
     <dgm:effectClrLst/>
     <dgm:txLinClrLst/>
@@ -691,13 +573,8 @@
     <dgm:fillClrLst meth="repeat">
       <a:schemeClr val="lt1"/>
     </dgm:fillClrLst>
-    <dgm:linClrLst>
-      <a:schemeClr val="accent5">
-        <a:shade val="80000"/>
-      </a:schemeClr>
-      <a:schemeClr val="accent5">
-        <a:tint val="70000"/>
-      </a:schemeClr>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
     </dgm:linClrLst>
     <dgm:effectClrLst/>
     <dgm:txLinClrLst/>
@@ -711,7 +588,7 @@
       <a:schemeClr val="lt1"/>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent5"/>
+      <a:schemeClr val="accent1"/>
     </dgm:linClrLst>
     <dgm:effectClrLst/>
     <dgm:txLinClrLst/>
@@ -725,7 +602,7 @@
       <a:schemeClr val="lt1"/>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent5"/>
+      <a:schemeClr val="accent1"/>
     </dgm:linClrLst>
     <dgm:effectClrLst/>
     <dgm:txLinClrLst/>
@@ -736,13 +613,13 @@
   </dgm:styleLbl>
   <dgm:styleLbl name="fgAccFollowNode1">
     <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent5">
+      <a:schemeClr val="accent1">
         <a:alpha val="90000"/>
         <a:tint val="40000"/>
       </a:schemeClr>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent5">
+      <a:schemeClr val="accent1">
         <a:alpha val="90000"/>
         <a:tint val="40000"/>
       </a:schemeClr>
@@ -756,13 +633,13 @@
   </dgm:styleLbl>
   <dgm:styleLbl name="alignAccFollowNode1">
     <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent5">
+      <a:schemeClr val="accent1">
         <a:alpha val="90000"/>
         <a:tint val="40000"/>
       </a:schemeClr>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent5">
+      <a:schemeClr val="accent1">
         <a:alpha val="90000"/>
         <a:tint val="40000"/>
       </a:schemeClr>
@@ -776,30 +653,15 @@
   </dgm:styleLbl>
   <dgm:styleLbl name="bgAccFollowNode1">
     <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent5">
+      <a:schemeClr val="accent1">
         <a:alpha val="90000"/>
         <a:tint val="40000"/>
       </a:schemeClr>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="dk1"/>
-    </dgm:txFillClrLst>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="fgAcc0">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="lt1">
+      <a:schemeClr val="accent1">
         <a:alpha val="90000"/>
-      </a:schemeClr>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent5">
-        <a:shade val="80000"/>
+        <a:tint val="40000"/>
       </a:schemeClr>
     </dgm:linClrLst>
     <dgm:effectClrLst/>
@@ -809,6 +671,22 @@
     </dgm:txFillClrLst>
     <dgm:txEffectClrLst/>
   </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc0">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="90000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
   <dgm:styleLbl name="fgAcc2">
     <dgm:fillClrLst meth="repeat">
       <a:schemeClr val="lt1">
@@ -816,9 +694,7 @@
       </a:schemeClr>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent5">
-        <a:tint val="99000"/>
-      </a:schemeClr>
+      <a:schemeClr val="accent1"/>
     </dgm:linClrLst>
     <dgm:effectClrLst/>
     <dgm:txLinClrLst/>
@@ -834,9 +710,7 @@
       </a:schemeClr>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent5">
-        <a:tint val="80000"/>
-      </a:schemeClr>
+      <a:schemeClr val="accent1"/>
     </dgm:linClrLst>
     <dgm:effectClrLst/>
     <dgm:txLinClrLst/>
@@ -852,9 +726,7 @@
       </a:schemeClr>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent5">
-        <a:tint val="70000"/>
-      </a:schemeClr>
+      <a:schemeClr val="accent1"/>
     </dgm:linClrLst>
     <dgm:effectClrLst/>
     <dgm:txLinClrLst/>
@@ -865,12 +737,12 @@
   </dgm:styleLbl>
   <dgm:styleLbl name="bgShp">
     <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent5">
+      <a:schemeClr val="accent1">
         <a:tint val="40000"/>
       </a:schemeClr>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="accent1"/>
     </dgm:linClrLst>
     <dgm:effectClrLst/>
     <dgm:txLinClrLst/>
@@ -881,12 +753,12 @@
   </dgm:styleLbl>
   <dgm:styleLbl name="dkBgShp">
     <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent5">
-        <a:shade val="90000"/>
+      <a:schemeClr val="accent1">
+        <a:shade val="80000"/>
       </a:schemeClr>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="accent1"/>
     </dgm:linClrLst>
     <dgm:effectClrLst/>
     <dgm:txLinClrLst/>
@@ -897,13 +769,13 @@
   </dgm:styleLbl>
   <dgm:styleLbl name="trBgShp">
     <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent5">
+      <a:schemeClr val="accent1">
         <a:tint val="50000"/>
         <a:alpha val="40000"/>
       </a:schemeClr>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent5"/>
+      <a:schemeClr val="accent1"/>
     </dgm:linClrLst>
     <dgm:effectClrLst/>
     <dgm:txLinClrLst/>
@@ -914,8 +786,8 @@
   </dgm:styleLbl>
   <dgm:styleLbl name="fgShp">
     <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent5">
-        <a:tint val="40000"/>
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
       </a:schemeClr>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
@@ -953,7 +825,7 @@
 <dgm:dataModel xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <dgm:ptLst>
     <dgm:pt modelId="{CE8BB443-F0BE-43DC-836C-1C7BC734525F}" type="doc">
-      <dgm:prSet loTypeId="urn:microsoft.com/office/officeart/2009/layout/CirclePictureHierarchy" loCatId="hierarchy" qsTypeId="urn:microsoft.com/office/officeart/2005/8/quickstyle/simple5" qsCatId="simple" csTypeId="urn:microsoft.com/office/officeart/2005/8/colors/accent5_3" csCatId="accent5" phldr="1"/>
+      <dgm:prSet loTypeId="urn:microsoft.com/office/officeart/2009/layout/CirclePictureHierarchy" loCatId="hierarchy" qsTypeId="urn:microsoft.com/office/officeart/2005/8/quickstyle/simple5" qsCatId="simple" csTypeId="urn:microsoft.com/office/officeart/2005/8/colors/accent1_2" csCatId="accent1" phldr="1"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -2221,7 +2093,7 @@
       </dgm:spPr>
     </dgm:pt>
     <dgm:pt modelId="{559922EE-4545-491E-B70C-0F9635934E8C}" type="pres">
-      <dgm:prSet presAssocID="{85A73317-70E2-43C1-B96B-3075618B937A}" presName="text4" presStyleLbl="revTx" presStyleIdx="10" presStyleCnt="22" custScaleX="76133" custLinFactNeighborX="-13905">
+      <dgm:prSet presAssocID="{85A73317-70E2-43C1-B96B-3075618B937A}" presName="text4" presStyleLbl="revTx" presStyleIdx="10" presStyleCnt="22" custScaleX="83534" custLinFactNeighborX="-9657">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -2263,7 +2135,7 @@
       </dgm:spPr>
     </dgm:pt>
     <dgm:pt modelId="{CE098FA8-6A37-4FBC-9FB7-077E9C84640D}" type="pres">
-      <dgm:prSet presAssocID="{3A0567DF-3917-4BB0-8CFF-15AC90CBB1D3}" presName="text4" presStyleLbl="revTx" presStyleIdx="11" presStyleCnt="22" custScaleX="88332" custLinFactNeighborX="-2729">
+      <dgm:prSet presAssocID="{3A0567DF-3917-4BB0-8CFF-15AC90CBB1D3}" presName="text4" presStyleLbl="revTx" presStyleIdx="11" presStyleCnt="22" custScaleX="110937" custLinFactNeighborX="2955">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -2347,7 +2219,7 @@
       </dgm:spPr>
     </dgm:pt>
     <dgm:pt modelId="{76CE45E1-3053-43B5-8665-5710DA88AC80}" type="pres">
-      <dgm:prSet presAssocID="{FE24A264-BEB4-40A0-AE0A-1069A48D0135}" presName="text4" presStyleLbl="revTx" presStyleIdx="13" presStyleCnt="22" custScaleX="103346" custScaleY="114395" custLinFactNeighborX="5024">
+      <dgm:prSet presAssocID="{FE24A264-BEB4-40A0-AE0A-1069A48D0135}" presName="text4" presStyleLbl="revTx" presStyleIdx="13" presStyleCnt="22" custScaleX="129815" custScaleY="81191" custLinFactNeighborX="12064">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -2515,7 +2387,7 @@
       </dgm:spPr>
     </dgm:pt>
     <dgm:pt modelId="{D4074FB4-BE76-4EFF-9379-4F56BAB0C90B}" type="pres">
-      <dgm:prSet presAssocID="{9C47766C-AB07-4114-9A5F-FF51ED2B0153}" presName="text4" presStyleLbl="revTx" presStyleIdx="17" presStyleCnt="22" custScaleX="82032" custLinFactNeighborX="-8976">
+      <dgm:prSet presAssocID="{9C47766C-AB07-4114-9A5F-FF51ED2B0153}" presName="text4" presStyleLbl="revTx" presStyleIdx="17" presStyleCnt="22" custScaleX="97964" custLinFactNeighborX="-1926">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -2557,7 +2429,7 @@
       </dgm:spPr>
     </dgm:pt>
     <dgm:pt modelId="{6B83B99B-54BF-4F3E-AA3B-A9F48439C5ED}" type="pres">
-      <dgm:prSet presAssocID="{3DCB5DB6-42F6-45C3-B8E4-39FEB580D1AA}" presName="text4" presStyleLbl="revTx" presStyleIdx="18" presStyleCnt="22" custScaleX="68439" custLinFactNeighborX="-12463">
+      <dgm:prSet presAssocID="{3DCB5DB6-42F6-45C3-B8E4-39FEB580D1AA}" presName="text4" presStyleLbl="revTx" presStyleIdx="18" presStyleCnt="22" custScaleX="85216" custLinFactNeighborX="-9643">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -2641,7 +2513,7 @@
       </dgm:spPr>
     </dgm:pt>
     <dgm:pt modelId="{A6257425-3A1D-4540-9C90-AE4B6BB7D4C7}" type="pres">
-      <dgm:prSet presAssocID="{471A75F3-E296-42DE-9CA3-E1B8D70291B5}" presName="text4" presStyleLbl="revTx" presStyleIdx="20" presStyleCnt="22" custScaleX="68960" custLinFactNeighborX="-14580">
+      <dgm:prSet presAssocID="{471A75F3-E296-42DE-9CA3-E1B8D70291B5}" presName="text4" presStyleLbl="revTx" presStyleIdx="20" presStyleCnt="22" custScaleX="85466" custLinFactNeighborX="-9028">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -2683,7 +2555,7 @@
       </dgm:spPr>
     </dgm:pt>
     <dgm:pt modelId="{29A5A7D5-5A8B-45F2-8153-934FE0FBE4E3}" type="pres">
-      <dgm:prSet presAssocID="{A62C05BE-FC11-49D0-9800-7F7E98FC69F1}" presName="text4" presStyleLbl="revTx" presStyleIdx="21" presStyleCnt="22" custScaleX="66603" custLinFactNeighborX="-13545">
+      <dgm:prSet presAssocID="{A62C05BE-FC11-49D0-9800-7F7E98FC69F1}" presName="text4" presStyleLbl="revTx" presStyleIdx="21" presStyleCnt="22" custScaleX="103007" custLinFactNeighborX="-979">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -2923,8 +2795,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="9839418" y="2978708"/>
-          <a:ext cx="483530" cy="110064"/>
+          <a:off x="8103914" y="2876472"/>
+          <a:ext cx="365682" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2935,16 +2807,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="0"/>
+                <a:pt x="0" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="55469"/>
+                <a:pt x="0" y="90060"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="483530" y="55469"/>
+                <a:pt x="365682" y="90060"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="483530" y="110064"/>
+                <a:pt x="365682" y="133703"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2952,8 +2824,8 @@
         <a:noFill/>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="accent5">
-              <a:tint val="70000"/>
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
               <a:hueOff val="0"/>
               <a:satOff val="0"/>
               <a:lumOff val="0"/>
@@ -2985,8 +2857,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="9443407" y="2978708"/>
-          <a:ext cx="396010" cy="110064"/>
+          <a:off x="7731933" y="2876472"/>
+          <a:ext cx="371981" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2997,16 +2869,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="396010" y="0"/>
+                <a:pt x="371981" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="396010" y="55469"/>
+                <a:pt x="371981" y="90060"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="55469"/>
+                <a:pt x="0" y="90060"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="110064"/>
+                <a:pt x="0" y="133703"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3014,8 +2886,8 @@
         <a:noFill/>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="accent5">
-              <a:tint val="70000"/>
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
               <a:hueOff val="0"/>
               <a:satOff val="0"/>
               <a:lumOff val="0"/>
@@ -3047,8 +2919,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="8953198" y="2519231"/>
-          <a:ext cx="886219" cy="110064"/>
+          <a:off x="7350650" y="2509176"/>
+          <a:ext cx="753264" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3059,16 +2931,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="0"/>
+                <a:pt x="0" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="55469"/>
+                <a:pt x="0" y="90060"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="886219" y="55469"/>
+                <a:pt x="753264" y="90060"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="886219" y="110064"/>
+                <a:pt x="753264" y="133703"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3076,8 +2948,8 @@
         <a:noFill/>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="accent5">
-              <a:tint val="80000"/>
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
               <a:hueOff val="0"/>
               <a:satOff val="0"/>
               <a:lumOff val="0"/>
@@ -3109,8 +2981,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="8066979" y="2978708"/>
-          <a:ext cx="498252" cy="110064"/>
+          <a:off x="6597386" y="2876472"/>
+          <a:ext cx="397407" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3121,16 +2993,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="0"/>
+                <a:pt x="0" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="55469"/>
+                <a:pt x="0" y="90060"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="498252" y="55469"/>
+                <a:pt x="397407" y="90060"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="498252" y="110064"/>
+                <a:pt x="397407" y="133703"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3138,8 +3010,8 @@
         <a:noFill/>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="accent5">
-              <a:tint val="70000"/>
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
               <a:hueOff val="0"/>
               <a:satOff val="0"/>
               <a:lumOff val="0"/>
@@ -3171,8 +3043,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="7651434" y="2978708"/>
-          <a:ext cx="415544" cy="110064"/>
+          <a:off x="6230949" y="2876472"/>
+          <a:ext cx="366437" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3183,16 +3055,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="415544" y="0"/>
+                <a:pt x="366437" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="415544" y="55469"/>
+                <a:pt x="366437" y="90060"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="55469"/>
+                <a:pt x="0" y="90060"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="110064"/>
+                <a:pt x="0" y="133703"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3200,8 +3072,8 @@
         <a:noFill/>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="accent5">
-              <a:tint val="70000"/>
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
               <a:hueOff val="0"/>
               <a:satOff val="0"/>
               <a:lumOff val="0"/>
@@ -3233,8 +3105,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="8066979" y="2519231"/>
-          <a:ext cx="886219" cy="110064"/>
+          <a:off x="6597386" y="2509176"/>
+          <a:ext cx="753264" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3245,16 +3117,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="886219" y="0"/>
+                <a:pt x="753264" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="886219" y="55469"/>
+                <a:pt x="753264" y="90060"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="55469"/>
+                <a:pt x="0" y="90060"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="110064"/>
+                <a:pt x="0" y="133703"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3262,8 +3134,8 @@
         <a:noFill/>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="accent5">
-              <a:tint val="80000"/>
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
               <a:hueOff val="0"/>
               <a:satOff val="0"/>
               <a:lumOff val="0"/>
@@ -3295,8 +3167,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5283514" y="2059753"/>
-          <a:ext cx="3669683" cy="110064"/>
+          <a:off x="4318482" y="2141880"/>
+          <a:ext cx="3032167" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3307,16 +3179,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="0"/>
+                <a:pt x="0" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="55469"/>
+                <a:pt x="0" y="90060"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="3669683" y="55469"/>
+                <a:pt x="3032167" y="90060"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="3669683" y="110064"/>
+                <a:pt x="3032167" y="133703"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3324,8 +3196,8 @@
         <a:noFill/>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="accent5">
-              <a:tint val="99000"/>
+            <a:schemeClr val="accent1">
+              <a:shade val="60000"/>
               <a:hueOff val="0"/>
               <a:satOff val="0"/>
               <a:lumOff val="0"/>
@@ -3357,8 +3229,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="6245502" y="2978708"/>
-          <a:ext cx="524604" cy="110064"/>
+          <a:off x="5079353" y="2876472"/>
+          <a:ext cx="447081" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3369,16 +3241,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="0"/>
+                <a:pt x="0" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="55469"/>
+                <a:pt x="0" y="90060"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="524604" y="55469"/>
+                <a:pt x="447081" y="90060"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="524604" y="110064"/>
+                <a:pt x="447081" y="133703"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3386,8 +3258,8 @@
         <a:noFill/>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="accent5">
-              <a:tint val="70000"/>
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
               <a:hueOff val="0"/>
               <a:satOff val="0"/>
               <a:lumOff val="0"/>
@@ -3419,8 +3291,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5800453" y="2978708"/>
-          <a:ext cx="445048" cy="135213"/>
+          <a:off x="4695867" y="2876472"/>
+          <a:ext cx="383486" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3431,16 +3303,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="445048" y="0"/>
+                <a:pt x="383486" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="445048" y="80618"/>
+                <a:pt x="383486" y="89362"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="80618"/>
+                <a:pt x="0" y="89362"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="135213"/>
+                <a:pt x="0" y="133005"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3448,8 +3320,8 @@
         <a:noFill/>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="accent5">
-              <a:tint val="70000"/>
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
               <a:hueOff val="0"/>
               <a:satOff val="0"/>
               <a:lumOff val="0"/>
@@ -3481,8 +3353,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5325595" y="2519231"/>
-          <a:ext cx="919906" cy="110064"/>
+          <a:off x="4314423" y="2509176"/>
+          <a:ext cx="764929" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3493,16 +3365,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="0"/>
+                <a:pt x="0" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="55469"/>
+                <a:pt x="0" y="90060"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="919906" y="55469"/>
+                <a:pt x="764929" y="90060"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="919906" y="110064"/>
+                <a:pt x="764929" y="133703"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3510,8 +3382,8 @@
         <a:noFill/>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="accent5">
-              <a:tint val="80000"/>
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
               <a:hueOff val="0"/>
               <a:satOff val="0"/>
               <a:lumOff val="0"/>
@@ -3543,8 +3415,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4405688" y="2978708"/>
-          <a:ext cx="464457" cy="110064"/>
+          <a:off x="3549494" y="2876472"/>
+          <a:ext cx="355352" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3555,16 +3427,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="0"/>
+                <a:pt x="0" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="55469"/>
+                <a:pt x="0" y="90060"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="464457" y="55469"/>
+                <a:pt x="355352" y="90060"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="464457" y="110064"/>
+                <a:pt x="355352" y="133703"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3572,8 +3444,8 @@
         <a:noFill/>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="accent5">
-              <a:tint val="70000"/>
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
               <a:hueOff val="0"/>
               <a:satOff val="0"/>
               <a:lumOff val="0"/>
@@ -3605,8 +3477,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3971808" y="2978708"/>
-          <a:ext cx="433880" cy="110064"/>
+          <a:off x="3171230" y="2876472"/>
+          <a:ext cx="378263" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3617,16 +3489,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="433880" y="0"/>
+                <a:pt x="378263" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="433880" y="55469"/>
+                <a:pt x="378263" y="90060"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="55469"/>
+                <a:pt x="0" y="90060"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="110064"/>
+                <a:pt x="0" y="133703"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3634,8 +3506,8 @@
         <a:noFill/>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="accent5">
-              <a:tint val="70000"/>
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
               <a:hueOff val="0"/>
               <a:satOff val="0"/>
               <a:lumOff val="0"/>
@@ -3667,8 +3539,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4405688" y="2519231"/>
-          <a:ext cx="919906" cy="110064"/>
+          <a:off x="3549494" y="2509176"/>
+          <a:ext cx="764929" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3679,16 +3551,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="919906" y="0"/>
+                <a:pt x="764929" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="919906" y="55469"/>
+                <a:pt x="764929" y="90060"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="55469"/>
+                <a:pt x="0" y="90060"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="110064"/>
+                <a:pt x="0" y="133703"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3696,8 +3568,8 @@
         <a:noFill/>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="accent5">
-              <a:tint val="80000"/>
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
               <a:hueOff val="0"/>
               <a:satOff val="0"/>
               <a:lumOff val="0"/>
@@ -3729,8 +3601,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5237794" y="2059753"/>
-          <a:ext cx="91440" cy="110064"/>
+          <a:off x="4268703" y="2141880"/>
+          <a:ext cx="91440" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3741,16 +3613,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="45720" y="0"/>
+                <a:pt x="49779" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="45720" y="55469"/>
+                <a:pt x="49779" y="90060"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="87800" y="55469"/>
+                <a:pt x="45720" y="90060"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="87800" y="110064"/>
+                <a:pt x="45720" y="133703"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3758,8 +3630,8 @@
         <a:noFill/>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="accent5">
-              <a:tint val="99000"/>
+            <a:schemeClr val="accent1">
+              <a:shade val="60000"/>
               <a:hueOff val="0"/>
               <a:satOff val="0"/>
               <a:lumOff val="0"/>
@@ -3791,8 +3663,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2564921" y="2978708"/>
-          <a:ext cx="500028" cy="110064"/>
+          <a:off x="2046596" y="2876472"/>
+          <a:ext cx="399711" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3803,16 +3675,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="0"/>
+                <a:pt x="0" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="55469"/>
+                <a:pt x="0" y="90060"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="500028" y="55469"/>
+                <a:pt x="399711" y="90060"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="500028" y="110064"/>
+                <a:pt x="399711" y="133703"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3820,8 +3692,8 @@
         <a:noFill/>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="accent5">
-              <a:tint val="70000"/>
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
               <a:hueOff val="0"/>
               <a:satOff val="0"/>
               <a:lumOff val="0"/>
@@ -3853,8 +3725,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2104065" y="2978708"/>
-          <a:ext cx="460855" cy="110064"/>
+          <a:off x="1678198" y="2876472"/>
+          <a:ext cx="368397" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3865,16 +3737,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="460855" y="0"/>
+                <a:pt x="368397" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="460855" y="55469"/>
+                <a:pt x="368397" y="90060"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="55469"/>
+                <a:pt x="0" y="90060"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="110064"/>
+                <a:pt x="0" y="133703"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3882,8 +3754,8 @@
         <a:noFill/>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="accent5">
-              <a:tint val="70000"/>
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
               <a:hueOff val="0"/>
               <a:satOff val="0"/>
               <a:lumOff val="0"/>
@@ -3915,8 +3787,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1613830" y="2519231"/>
-          <a:ext cx="951091" cy="110064"/>
+          <a:off x="1286315" y="2509176"/>
+          <a:ext cx="760281" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3927,16 +3799,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="0"/>
+                <a:pt x="0" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="55469"/>
+                <a:pt x="0" y="90060"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="951091" y="55469"/>
+                <a:pt x="760281" y="90060"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="951091" y="110064"/>
+                <a:pt x="760281" y="133703"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3944,8 +3816,8 @@
         <a:noFill/>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="accent5">
-              <a:tint val="80000"/>
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
               <a:hueOff val="0"/>
               <a:satOff val="0"/>
               <a:lumOff val="0"/>
@@ -3977,8 +3849,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="662739" y="2978708"/>
-          <a:ext cx="480442" cy="110064"/>
+          <a:off x="526034" y="2876472"/>
+          <a:ext cx="384054" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3989,16 +3861,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="0"/>
+                <a:pt x="0" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="55469"/>
+                <a:pt x="0" y="90060"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="480442" y="55469"/>
+                <a:pt x="384054" y="90060"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="480442" y="110064"/>
+                <a:pt x="384054" y="133703"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -4006,8 +3878,8 @@
         <a:noFill/>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="accent5">
-              <a:tint val="70000"/>
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
               <a:hueOff val="0"/>
               <a:satOff val="0"/>
               <a:lumOff val="0"/>
@@ -4039,8 +3911,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="182297" y="2978708"/>
-          <a:ext cx="480442" cy="110064"/>
+          <a:off x="141979" y="2876472"/>
+          <a:ext cx="384054" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4051,16 +3923,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="480442" y="0"/>
+                <a:pt x="384054" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="480442" y="55469"/>
+                <a:pt x="384054" y="90060"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="55469"/>
+                <a:pt x="0" y="90060"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="110064"/>
+                <a:pt x="0" y="133703"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -4068,8 +3940,8 @@
         <a:noFill/>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="accent5">
-              <a:tint val="70000"/>
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
               <a:hueOff val="0"/>
               <a:satOff val="0"/>
               <a:lumOff val="0"/>
@@ -4101,8 +3973,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="662739" y="2519231"/>
-          <a:ext cx="951091" cy="110064"/>
+          <a:off x="526034" y="2509176"/>
+          <a:ext cx="760281" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4113,16 +3985,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="951091" y="0"/>
+                <a:pt x="760281" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="951091" y="55469"/>
+                <a:pt x="760281" y="90060"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="55469"/>
+                <a:pt x="0" y="90060"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="110064"/>
+                <a:pt x="0" y="133703"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -4130,8 +4002,8 @@
         <a:noFill/>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="accent5">
-              <a:tint val="80000"/>
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
               <a:hueOff val="0"/>
               <a:satOff val="0"/>
               <a:lumOff val="0"/>
@@ -4163,8 +4035,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1613830" y="2059753"/>
-          <a:ext cx="3669683" cy="110064"/>
+          <a:off x="1286315" y="2141880"/>
+          <a:ext cx="3032167" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4175,16 +4047,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="3669683" y="0"/>
+                <a:pt x="3032167" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="3669683" y="55469"/>
+                <a:pt x="3032167" y="90060"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="55469"/>
+                <a:pt x="0" y="90060"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="110064"/>
+                <a:pt x="0" y="133703"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -4192,8 +4064,8 @@
         <a:noFill/>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="accent5">
-              <a:tint val="99000"/>
+            <a:schemeClr val="accent1">
+              <a:shade val="60000"/>
               <a:hueOff val="0"/>
               <a:satOff val="0"/>
               <a:lumOff val="0"/>
@@ -4225,8 +4097,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5108808" y="1710341"/>
-          <a:ext cx="349412" cy="349412"/>
+          <a:off x="4178826" y="1908287"/>
+          <a:ext cx="279312" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -4277,8 +4149,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5458220" y="1709467"/>
-          <a:ext cx="524118" cy="349412"/>
+          <a:off x="4458139" y="1907589"/>
+          <a:ext cx="418968" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4326,8 +4198,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="5458220" y="1709467"/>
-        <a:ext cx="524118" cy="349412"/>
+        <a:off x="4458139" y="1907589"/>
+        <a:ext cx="418968" cy="279312"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{9C31D818-38CA-4F31-872B-514D0F946B3C}">
@@ -4337,8 +4209,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1439124" y="2169818"/>
-          <a:ext cx="349412" cy="349412"/>
+          <a:off x="1146658" y="2275583"/>
+          <a:ext cx="279312" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -4389,8 +4261,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1788536" y="2168945"/>
-          <a:ext cx="524118" cy="349412"/>
+          <a:off x="1425971" y="2274885"/>
+          <a:ext cx="418968" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4438,8 +4310,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1788536" y="2168945"/>
-        <a:ext cx="524118" cy="349412"/>
+        <a:off x="1425971" y="2274885"/>
+        <a:ext cx="418968" cy="279312"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{1250F72D-60DB-43B0-834A-5EA96D96D80F}">
@@ -4449,8 +4321,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="488033" y="2629296"/>
-          <a:ext cx="349412" cy="349412"/>
+          <a:off x="386377" y="2642879"/>
+          <a:ext cx="279312" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -4501,8 +4373,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="837445" y="2628422"/>
-          <a:ext cx="524118" cy="349412"/>
+          <a:off x="665690" y="2642181"/>
+          <a:ext cx="418968" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4550,8 +4422,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="837445" y="2628422"/>
-        <a:ext cx="524118" cy="349412"/>
+        <a:off x="665690" y="2642181"/>
+        <a:ext cx="418968" cy="279312"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{6F392430-3A4B-4377-99E5-2B841107A9A2}">
@@ -4561,8 +4433,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="7591" y="3088773"/>
-          <a:ext cx="349412" cy="349412"/>
+          <a:off x="2322" y="3010175"/>
+          <a:ext cx="279312" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -4613,8 +4485,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="357003" y="3087899"/>
-          <a:ext cx="524118" cy="349412"/>
+          <a:off x="281635" y="3009477"/>
+          <a:ext cx="418968" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4662,8 +4534,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="357003" y="3087899"/>
-        <a:ext cx="524118" cy="349412"/>
+        <a:off x="281635" y="3009477"/>
+        <a:ext cx="418968" cy="279312"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{06617EAB-A912-4FFB-8349-3E44430D3112}">
@@ -4673,8 +4545,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="968475" y="3088773"/>
-          <a:ext cx="349412" cy="349412"/>
+          <a:off x="770432" y="3010175"/>
+          <a:ext cx="279312" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -4725,8 +4597,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1317887" y="3087899"/>
-          <a:ext cx="524118" cy="349412"/>
+          <a:off x="1049745" y="3009477"/>
+          <a:ext cx="418968" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4774,8 +4646,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1317887" y="3087899"/>
-        <a:ext cx="524118" cy="349412"/>
+        <a:off x="1049745" y="3009477"/>
+        <a:ext cx="418968" cy="279312"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{41BBEB59-EF70-4AEA-9881-EB5BF6EE3538}">
@@ -4785,8 +4657,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2375362" y="2629296"/>
-          <a:ext cx="379119" cy="349412"/>
+          <a:off x="1895066" y="2642879"/>
+          <a:ext cx="303059" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -4837,8 +4709,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2757489" y="2628422"/>
-          <a:ext cx="524118" cy="349412"/>
+          <a:off x="2200531" y="2642181"/>
+          <a:ext cx="418968" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4886,8 +4758,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2757489" y="2628422"/>
-        <a:ext cx="524118" cy="349412"/>
+        <a:off x="2200531" y="2642181"/>
+        <a:ext cx="418968" cy="279312"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{EA21AC87-C4DC-4853-9264-DC2EBF7A7DFD}">
@@ -4897,8 +4769,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1929359" y="3088773"/>
-          <a:ext cx="349412" cy="349412"/>
+          <a:off x="1538542" y="3010175"/>
+          <a:ext cx="279312" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -4949,8 +4821,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2278772" y="3087899"/>
-          <a:ext cx="524118" cy="349412"/>
+          <a:off x="1817854" y="3009477"/>
+          <a:ext cx="418968" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4998,8 +4870,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2278772" y="3087899"/>
-        <a:ext cx="524118" cy="349412"/>
+        <a:off x="1817854" y="3009477"/>
+        <a:ext cx="418968" cy="279312"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{FC1DFEE3-2398-4E16-AE3D-4F2635645B02}">
@@ -5009,8 +4881,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2890243" y="3088773"/>
-          <a:ext cx="349412" cy="349412"/>
+          <a:off x="2306651" y="3010175"/>
+          <a:ext cx="279312" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -5061,8 +4933,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3240096" y="3087899"/>
-          <a:ext cx="416066" cy="349412"/>
+          <a:off x="2586316" y="3009477"/>
+          <a:ext cx="332594" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5110,8 +4982,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3240096" y="3087899"/>
-        <a:ext cx="416066" cy="349412"/>
+        <a:off x="2586316" y="3009477"/>
+        <a:ext cx="332594" cy="279312"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{FE90BA29-306C-4AB5-9943-DA8459E09443}">
@@ -5121,8 +4993,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5150889" y="2169818"/>
-          <a:ext cx="349412" cy="349412"/>
+          <a:off x="4174767" y="2275583"/>
+          <a:ext cx="279312" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -5173,8 +5045,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5500301" y="2168945"/>
-          <a:ext cx="524118" cy="349412"/>
+          <a:off x="4454080" y="2274885"/>
+          <a:ext cx="418968" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5222,8 +5094,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="5500301" y="2168945"/>
-        <a:ext cx="524118" cy="349412"/>
+        <a:off x="4454080" y="2274885"/>
+        <a:ext cx="418968" cy="279312"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{FB71D438-1DB2-4E92-A4B5-676418847572}">
@@ -5233,8 +5105,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4230982" y="2629296"/>
-          <a:ext cx="349412" cy="349412"/>
+          <a:off x="3409837" y="2642879"/>
+          <a:ext cx="279312" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -5285,8 +5157,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4580395" y="2628422"/>
-          <a:ext cx="524118" cy="349412"/>
+          <a:off x="3689150" y="2642181"/>
+          <a:ext cx="418968" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5334,8 +5206,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4580395" y="2628422"/>
-        <a:ext cx="524118" cy="349412"/>
+        <a:off x="3689150" y="2642181"/>
+        <a:ext cx="418968" cy="279312"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{26773E47-B122-45D3-855E-B793488FF916}">
@@ -5345,8 +5217,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3797101" y="3088773"/>
-          <a:ext cx="349412" cy="349412"/>
+          <a:off x="3031574" y="3010175"/>
+          <a:ext cx="279312" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -5397,8 +5269,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4136181" y="3087899"/>
-          <a:ext cx="399027" cy="349412"/>
+          <a:off x="3304920" y="3009477"/>
+          <a:ext cx="349981" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5446,8 +5318,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4136181" y="3087899"/>
-        <a:ext cx="399027" cy="349412"/>
+        <a:off x="3304920" y="3009477"/>
+        <a:ext cx="349981" cy="279312"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{573EDEF5-5CD1-41FF-ACBE-3DF79E8F3D63}">
@@ -5457,8 +5329,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4695440" y="3088773"/>
-          <a:ext cx="349412" cy="349412"/>
+          <a:off x="3765190" y="3010175"/>
+          <a:ext cx="279312" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -5509,8 +5381,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5061126" y="3087899"/>
-          <a:ext cx="462964" cy="349412"/>
+          <a:off x="4033972" y="3009477"/>
+          <a:ext cx="464791" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5559,8 +5431,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="5061126" y="3087899"/>
-        <a:ext cx="462964" cy="349412"/>
+        <a:off x="4033972" y="3009477"/>
+        <a:ext cx="464791" cy="279312"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{148A9995-87EC-442A-BF71-CEDE53EA2019}">
@@ -5570,8 +5442,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="6070795" y="2629296"/>
-          <a:ext cx="349412" cy="349412"/>
+          <a:off x="4939697" y="2642879"/>
+          <a:ext cx="279312" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -5622,8 +5494,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="6420208" y="2628422"/>
-          <a:ext cx="524118" cy="349412"/>
+          <a:off x="5219009" y="2642181"/>
+          <a:ext cx="418968" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5671,8 +5543,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="6420208" y="2628422"/>
-        <a:ext cx="524118" cy="349412"/>
+        <a:off x="5219009" y="2642181"/>
+        <a:ext cx="418968" cy="279312"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{4F024B8E-5D77-44F1-B629-61CD8E2D6DD0}">
@@ -5682,8 +5554,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5625747" y="3113922"/>
-          <a:ext cx="349412" cy="349412"/>
+          <a:off x="4556211" y="3009477"/>
+          <a:ext cx="279312" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -5734,8 +5606,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5992723" y="3087899"/>
-          <a:ext cx="541655" cy="399710"/>
+          <a:off x="4823610" y="3035047"/>
+          <a:ext cx="543884" cy="226776"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5784,8 +5656,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="5992723" y="3087899"/>
-        <a:ext cx="541655" cy="399710"/>
+        <a:off x="4823610" y="3035047"/>
+        <a:ext cx="543884" cy="226776"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{8C851992-24F3-4B62-BB29-6CA271940DAF}">
@@ -5795,8 +5667,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="6595400" y="3088773"/>
-          <a:ext cx="349412" cy="349412"/>
+          <a:off x="5386778" y="3010175"/>
+          <a:ext cx="279312" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -5847,8 +5719,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="6957475" y="3087899"/>
-          <a:ext cx="365006" cy="349412"/>
+          <a:off x="5676213" y="3009477"/>
+          <a:ext cx="291778" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5897,8 +5769,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="6957475" y="3087899"/>
-        <a:ext cx="365006" cy="349412"/>
+        <a:off x="5676213" y="3009477"/>
+        <a:ext cx="291778" cy="279312"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{87D3AC67-E8C0-4DD3-AF56-A54675796D39}">
@@ -5908,8 +5780,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="8778492" y="2169818"/>
-          <a:ext cx="349412" cy="349412"/>
+          <a:off x="7210994" y="2275583"/>
+          <a:ext cx="279312" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -5960,8 +5832,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="9127904" y="2168945"/>
-          <a:ext cx="524118" cy="349412"/>
+          <a:off x="7490306" y="2274885"/>
+          <a:ext cx="418968" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6009,8 +5881,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="9127904" y="2168945"/>
-        <a:ext cx="524118" cy="349412"/>
+        <a:off x="7490306" y="2274885"/>
+        <a:ext cx="418968" cy="279312"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{9D71F757-A244-4130-80E7-9F8318DBB160}">
@@ -6020,8 +5892,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="7892272" y="2629296"/>
-          <a:ext cx="349412" cy="349412"/>
+          <a:off x="6457730" y="2642879"/>
+          <a:ext cx="279312" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -6072,8 +5944,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="8241685" y="2628422"/>
-          <a:ext cx="524118" cy="349412"/>
+          <a:off x="6737042" y="2642181"/>
+          <a:ext cx="418968" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6121,8 +5993,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="8241685" y="2628422"/>
-        <a:ext cx="524118" cy="349412"/>
+        <a:off x="6737042" y="2642181"/>
+        <a:ext cx="418968" cy="279312"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{B5516094-8002-4561-835D-8A1E31A99B4A}">
@@ -6132,8 +6004,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="7476728" y="3088773"/>
-          <a:ext cx="349412" cy="349412"/>
+          <a:off x="6091293" y="3010175"/>
+          <a:ext cx="279312" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -6184,8 +6056,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="7826182" y="3087899"/>
-          <a:ext cx="429945" cy="349412"/>
+          <a:off x="6366801" y="3009477"/>
+          <a:ext cx="410438" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6234,8 +6106,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="7826182" y="3087899"/>
-        <a:ext cx="429945" cy="349412"/>
+        <a:off x="6366801" y="3009477"/>
+        <a:ext cx="410438" cy="279312"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{D09ADDAA-7C47-404F-B5F5-44E87A97673F}">
@@ -6245,8 +6117,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="8390525" y="3088773"/>
-          <a:ext cx="349412" cy="349412"/>
+          <a:off x="6855137" y="3010175"/>
+          <a:ext cx="279312" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -6297,8 +6169,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="8757325" y="3087899"/>
-          <a:ext cx="358701" cy="349412"/>
+          <a:off x="7125019" y="3009477"/>
+          <a:ext cx="357028" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6347,8 +6219,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="8757325" y="3087899"/>
-        <a:ext cx="358701" cy="349412"/>
+        <a:off x="7125019" y="3009477"/>
+        <a:ext cx="357028" cy="279312"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{EBD4C9B2-EDC4-4292-BB42-6C954E705E13}">
@@ -6358,8 +6230,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="9664712" y="2629296"/>
-          <a:ext cx="349412" cy="349412"/>
+          <a:off x="7964258" y="2642879"/>
+          <a:ext cx="279312" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -6410,8 +6282,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="10014124" y="2628422"/>
-          <a:ext cx="524118" cy="349412"/>
+          <a:off x="8243570" y="2642181"/>
+          <a:ext cx="418968" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6459,8 +6331,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="10014124" y="2628422"/>
-        <a:ext cx="524118" cy="349412"/>
+        <a:off x="8243570" y="2642181"/>
+        <a:ext cx="418968" cy="279312"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{740876E6-F5BF-40DC-BCAF-A91ED8FBB918}">
@@ -6470,8 +6342,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="9268701" y="3088773"/>
-          <a:ext cx="349412" cy="349412"/>
+          <a:off x="7592277" y="3010175"/>
+          <a:ext cx="279312" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -6522,8 +6394,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="9623040" y="3087899"/>
-          <a:ext cx="361432" cy="349412"/>
+          <a:off x="7864211" y="3009477"/>
+          <a:ext cx="358075" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6572,8 +6444,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="9623040" y="3087899"/>
-        <a:ext cx="361432" cy="349412"/>
+        <a:off x="7864211" y="3009477"/>
+        <a:ext cx="358075" cy="279312"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{49C7AFDA-958E-4DD9-8AAB-958FA03F032A}">
@@ -6583,8 +6455,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="10148242" y="3088773"/>
-          <a:ext cx="349412" cy="349412"/>
+          <a:off x="8329940" y="3010175"/>
+          <a:ext cx="279312" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -6635,8 +6507,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="10514183" y="3087899"/>
-          <a:ext cx="349078" cy="349412"/>
+          <a:off x="8598852" y="3009477"/>
+          <a:ext cx="431567" cy="279312"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6685,8 +6557,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="10514183" y="3087899"/>
-        <a:ext cx="349078" cy="349412"/>
+        <a:off x="8598852" y="3009477"/>
+        <a:ext cx="431567" cy="279312"/>
       </dsp:txXfrm>
     </dsp:sp>
   </dsp:spTree>
@@ -8293,13 +8165,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>160733</xdr:colOff>
+      <xdr:colOff>160734</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>41672</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>172640</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>89297</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
@@ -8629,7 +8501,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>